<commit_message>
Add song selected transition effect(not done yet..
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Songs/2-World Wide Web/Chart4.xlsx
+++ b/Assets/StreamingAssets/Songs/2-World Wide Web/Chart4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\StreamingAssets\Songs\World Wide Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xenody-main\Assets\StreamingAssets\Songs\2-World Wide Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E23CE-91BC-473E-AD78-E95349A5C597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC85DEEF-57A9-413D-A852-E37FBA5F18F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="speed" sheetId="7" r:id="rId1"/>
@@ -135,14 +135,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#63b8ff</t>
-  </si>
-  <si>
     <t>Jagnum</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#f0ffff</t>
   </si>
   <si>
     <t>sp</t>
@@ -174,6 +168,14 @@
   </si>
   <si>
     <t>EndUcolor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#82e300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#f5ffe7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -230,7 +232,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -241,6 +243,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9C96A9-1D89-4E37-B465-2098CA6EFD66}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -573,7 +581,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -581,24 +589,80 @@
         <v>0</v>
       </c>
       <c r="B2">
+        <v>137.01499999999999</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>137.01499999999999</v>
+      </c>
+      <c r="B3">
+        <v>137.48400000000001</v>
+      </c>
+      <c r="C3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>137.48400000000001</v>
+      </c>
+      <c r="B4">
+        <v>137.953</v>
+      </c>
+      <c r="C4">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>137.953</v>
+      </c>
+      <c r="B5">
+        <v>138.42099999999999</v>
+      </c>
+      <c r="C5">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>138.42099999999999</v>
+      </c>
+      <c r="B6">
+        <v>138.88999999999999</v>
+      </c>
+      <c r="C6">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>138.88999999999999</v>
+      </c>
+      <c r="B7">
         <v>999</v>
       </c>
-      <c r="C2">
+      <c r="C7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FB3F29-4751-4825-9A13-CD8F2FFC98B2}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -611,16 +675,16 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -630,16 +694,20 @@
       <c r="B2">
         <v>154.828</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
+      <c r="C2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C10" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2644,8 +2712,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D668"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView topLeftCell="A593" workbookViewId="0">
+      <selection activeCell="A621" sqref="A621"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12014,8 +12082,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12052,7 +12120,7 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -21546,13 +21614,13 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
         <v>31</v>
-      </c>
-      <c r="L1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>